<commit_message>
Update Excel export template cell mappings
Revised cell mappings to match updated Excel templates:

SEM/Social Template:
- Flight Start: C3
- Flight End: C4
- Total Budget: C5
- Line Item Range: B12:D49 (unchanged)

Programmatic Template:
- Total Budget: C4 (was C4)
- Total Impressions: C5 (was C5)
- CPM: C6 (added)
- Flight Start: F3 (unchanged)
- Flight End: F4 (unchanged)
- Line Item Range: C13:G52 (removed column B)

YouTube Template:
- Total Budget: C4 (unchanged)
- Impressions/Views: C5 (unchanged)
- CPM/CPV: C6 (unchanged)
- Flight Start: F4 (unchanged)
- Flight End: F5 (unchanged)
- Line Item Range: unchanged

All mappings now correctly populate revised template cells.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/SEM_Social Budget Flighting Template.xlsx
+++ b/templates/SEM_Social Budget Flighting Template.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29325"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2376BFB-0EAA-4675-B2D7-95A122D263F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="SEM + Social Template" sheetId="1" r:id="rId4"/>
+    <sheet name="SEM + Social Template" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>For multiple LI orders label excel tabs appropriately</t>
   </si>
@@ -19,10 +39,10 @@
     <t>Flight Start</t>
   </si>
   <si>
-    <t>Total Budget</t>
+    <t>Flight End</t>
   </si>
   <si>
-    <t>Flight End</t>
+    <t>Total Budget</t>
   </si>
   <si>
     <t>Even Monthly (Y/N)</t>
@@ -32,9 +52,6 @@
   </si>
   <si>
     <t>Monthly Budget Flighting</t>
-  </si>
-  <si>
-    <t>Custom Budget Flighting</t>
   </si>
   <si>
     <t>Flight Check:</t>
@@ -52,59 +69,61 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
-      <sz val="12.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -124,22 +143,20 @@
         <bgColor rgb="FFE7E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
-    <border/>
+  <borders count="18">
     <border>
       <left/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -154,124 +171,125 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <top style="medium">
+      <right/>
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="medium">
+      <left/>
+      <right/>
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -280,6 +298,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -288,6 +307,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -298,6 +318,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -306,6 +327,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -316,100 +338,107 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="14" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="3" fontId="4" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="3" fontId="7" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="17" fillId="0" fontId="7" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="18" fillId="4" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="4" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="4" fontId="7" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="19" fillId="4" fontId="7" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="17" fillId="4" fontId="7" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="20" fillId="4" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="21" fillId="4" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="21" fillId="4" fontId="7" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="22" fillId="4" fontId="7" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <color rgb="FF385623"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
       <font>
@@ -421,84 +450,74 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color rgb="FF385623"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7E6E6"/>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFFFF"/>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFE7E6E6"/>
-          <bgColor rgb="FFE7E6E6"/>
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="SEM + Social Template-style">
-      <tableStyleElement dxfId="4" type="headerRow"/>
-      <tableStyleElement dxfId="4" type="firstRowStripe"/>
-      <tableStyleElement dxfId="5" type="secondRowStripe"/>
+    <tableStyle name="SEM + Social Template-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B10:G48" displayName="Table_1" name="Table_1" id="1">
-  <tableColumns count="6">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B11:D49">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Start"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="End"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Budget"/>
   </tableColumns>
-  <tableStyleInfo name="SEM + Social Template-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
+  <tableStyleInfo name="SEM + Social Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -514,40 +533,40 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0563C1"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -688,455 +707,305 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D1015"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:D34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="2.0"/>
-    <col customWidth="1" min="2" max="2" width="15.5"/>
-    <col customWidth="1" min="3" max="3" width="14.0"/>
-    <col customWidth="1" min="4" max="4" width="12.13"/>
-    <col customWidth="1" min="5" max="5" width="17.75"/>
-    <col customWidth="1" min="6" max="7" width="11.25"/>
-    <col customWidth="1" min="8" max="26" width="7.63"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="23" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="18.0" customHeight="1">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" ht="18.0" customHeight="1">
-      <c r="B4" s="6" t="s">
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:4" ht="18" customHeight="1">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="18" customHeight="1">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" ht="18.0" customHeight="1">
-      <c r="B5" s="4"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="18" customHeight="1">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="C6" s="21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" ht="18.0" customHeight="1">
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" ht="33.75" customHeight="1">
-      <c r="B8" s="11" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="18" customHeight="1">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="33.75" customHeight="1">
+      <c r="B9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="B9" s="14" t="s">
+      <c r="C10" s="5" t="str">
+        <f>IF($C$6="N","",IF(B12=$C$3,IF(MAX(C12:C57)=$C$4,"Good","Wrong Date"),"Wrong Date"))</f>
+        <v>Good</v>
+      </c>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="15" t="str">
-        <f>IF($F$5="N","",IF(B11=$F$3,IF(MAX(C11:C56)=$F$4,"Good","Wrong Date"),"Wrong Date"))</f>
-        <v>Good</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="15" t="str">
-        <f>IF($F$5="Y","",IF(E11=$F$3,IF(MAX(F11:F56)=$F$4,"Good","Wrong Date"),"Wrong Date"))</f>
-        <v/>
-      </c>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="B10" s="18" t="s">
+      <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="24"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="28"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="24"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="28"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="24"/>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="28"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="24"/>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="28"/>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="24"/>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="28"/>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="24"/>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="28"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="33"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="33"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="33"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="33"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="33"/>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="33"/>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="33"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="33"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="33"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="33"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="33"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="33"/>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="24"/>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="B36" s="25"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="28"/>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="24"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="28"/>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="24"/>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="B40" s="25"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="28"/>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="B41" s="21"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="24"/>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="B42" s="25"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="28"/>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="B43" s="21"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="24"/>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="28"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="B45" s="21"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="24"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="B46" s="25"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="28"/>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="B47" s="21"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="24"/>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="B48" s="34"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="37"/>
-    </row>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B12" s="22"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B14" s="22"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="23"/>
+    </row>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B16" s="22"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B18" s="22"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B20" s="22"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="23"/>
+    </row>
+    <row r="21" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B22" s="22"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="23"/>
+    </row>
+    <row r="23" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B24" s="24"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B25" s="10"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B26" s="24"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B27" s="10"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B28" s="24"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B29" s="10"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B30" s="24"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B31" s="10"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B32" s="24"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B33" s="10"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B34" s="24"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="25"/>
+    </row>
+    <row r="35" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B35" s="10"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="16"/>
+    </row>
+    <row r="36" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B36" s="22"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="16"/>
+    </row>
+    <row r="38" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B38" s="22"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="23"/>
+    </row>
+    <row r="39" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="16"/>
+    </row>
+    <row r="40" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B40" s="22"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="23"/>
+    </row>
+    <row r="41" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B41" s="10"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="16"/>
+    </row>
+    <row r="42" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B42" s="22"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="23"/>
+    </row>
+    <row r="43" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B44" s="22"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="23"/>
+    </row>
+    <row r="45" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B46" s="22"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="23"/>
+    </row>
+    <row r="47" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="16"/>
+    </row>
+    <row r="48" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B48" s="22"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="23"/>
+    </row>
+    <row r="49" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B49" s="12"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="51" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="52" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="53" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="54" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="55" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="56" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="57" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="58" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="59" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="60" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="61" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="62" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="63" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="64" spans="2:4" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2087,53 +1956,31 @@
     <row r="1012" ht="14.25" customHeight="1"/>
     <row r="1013" ht="14.25" customHeight="1"/>
     <row r="1014" ht="14.25" customHeight="1"/>
+    <row r="1015" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B9:D9"/>
   </mergeCells>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH(("wrong"),(C9))))</formula>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="wrong">
+      <formula>NOT(ISERROR(SEARCH(("wrong"),(C10))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+  <conditionalFormatting sqref="C10">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH(("good"),(C9))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("good"),(C10))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="INCORRECT">
-      <formula>NOT(ISERROR(SEARCH(("INCORRECT"),(G9))))</formula>
+  <conditionalFormatting sqref="B9:D9">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
-      <formula>"Good"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="wrong">
-      <formula>NOT(ISERROR(SEARCH(("wrong"),(F9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="good">
-      <formula>NOT(ISERROR(SEARCH(("good"),(F9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:G8">
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>$G$10="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>